<commit_message>
small changes on enum values
</commit_message>
<xml_diff>
--- a/template_examples/blood_dna_template.xlsx
+++ b/template_examples/blood_dna_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pavel/code/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCC596BF-F0FC-AC43-AB55-99D5D73C83FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AE8450D-1D1F-924E-9AD7-9243D31119C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -672,9 +672,6 @@
     <t>Comments</t>
   </si>
   <si>
-    <t>Olink</t>
-  </si>
-  <si>
     <t>USPS</t>
   </si>
   <si>
@@ -693,9 +690,6 @@
     <t>ship to</t>
   </si>
   <si>
-    <t>Adaptive Biotechnologies</t>
-  </si>
-  <si>
     <t>Baseline</t>
   </si>
   <si>
@@ -880,6 +874,12 @@
   </si>
   <si>
     <t>Ice_Pack</t>
+  </si>
+  <si>
+    <t>WES</t>
+  </si>
+  <si>
+    <t>MDA_Bernatchez</t>
   </si>
 </sst>
 </file>
@@ -1463,7 +1463,7 @@
   <dimension ref="A1:F218"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -1492,7 +1492,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -1506,7 +1506,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -1534,7 +1534,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>45</v>
+        <v>113</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -1548,7 +1548,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>52</v>
+        <v>114</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -1562,7 +1562,7 @@
         <v>8</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -1576,7 +1576,7 @@
         <v>9</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -1590,7 +1590,7 @@
         <v>10</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -1604,7 +1604,7 @@
         <v>11</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -1629,7 +1629,7 @@
         <v>2</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C12" s="3">
         <v>37539</v>
@@ -1646,7 +1646,7 @@
         <v>13</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -1660,7 +1660,7 @@
         <v>14</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -1674,7 +1674,7 @@
         <v>15</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -2694,7 +2694,7 @@
       <formula1>"1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,Not Reported,Other"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{5F8B2AEC-EDE5-C44B-A714-783B06DCAC87}">
-      <formula1>"Olink,Not Reported,Other"</formula1>
+      <formula1>"Olink,Not Reported,Other,WES"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10" xr:uid="{0D19CD82-2118-DA4F-84DD-8D7D25E5E47B}">
       <formula1>"Frozen_Dry_Ice,Frozen_Shipper,Ice_Pack,Ambient,Not Reported,Other"</formula1>
@@ -2709,7 +2709,7 @@
       <formula1>"FEDEX,USPS,UPC"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6" xr:uid="{D81C2091-8E55-1248-9AD1-250272DBC233}">
-      <formula1>"MDA_CIMAC,MSSM_CIMAC,STAN_CIMAC,DFCI_CIMAC,Broad_CIMAC,FNLCR_MoCha,Nationwide Children's Hospital,Adaptive Biotechnologies,Not Reported,Other"</formula1>
+      <formula1>"MDA_Bernatchez,Nationwide Children's Hospital,Adaptive Biotechnologies,Not Reported,Other"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2842,31 +2842,31 @@
         <v>35</v>
       </c>
       <c r="Q2" s="8" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="R2" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="S2" s="8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="T2" s="8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="U2" s="8" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="V2" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="W2" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="X2" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="Y2" s="9" t="s">
         <v>109</v>
-      </c>
-      <c r="X2" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="Y2" s="9" t="s">
-        <v>111</v>
       </c>
       <c r="Z2" s="2" t="s">
         <v>36</v>
@@ -2904,64 +2904,64 @@
         <v>1</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="F3" t="s">
         <v>53</v>
       </c>
-      <c r="D3" t="s">
+      <c r="G3" t="s">
         <v>54</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="F3" t="s">
-        <v>55</v>
-      </c>
-      <c r="G3" t="s">
-        <v>56</v>
-      </c>
       <c r="H3" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3" t="s">
+        <v>55</v>
+      </c>
+      <c r="K3" t="s">
+        <v>56</v>
+      </c>
+      <c r="L3" t="s">
+        <v>85</v>
+      </c>
+      <c r="M3" t="s">
+        <v>86</v>
+      </c>
+      <c r="N3" t="s">
         <v>57</v>
-      </c>
-      <c r="K3" t="s">
-        <v>58</v>
-      </c>
-      <c r="L3" t="s">
-        <v>87</v>
-      </c>
-      <c r="M3" t="s">
-        <v>88</v>
-      </c>
-      <c r="N3" t="s">
-        <v>59</v>
       </c>
       <c r="O3">
         <v>1</v>
       </c>
       <c r="P3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="Q3">
         <v>1</v>
       </c>
       <c r="R3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="S3" s="7">
         <v>1</v>
       </c>
       <c r="T3" s="7" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="U3" s="7">
         <v>1</v>
       </c>
       <c r="V3" s="7" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="W3" s="10">
         <v>9</v>
@@ -2976,28 +2976,28 @@
         <v>1</v>
       </c>
       <c r="AA3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="AB3">
         <v>0</v>
       </c>
       <c r="AC3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE3" t="s">
         <v>61</v>
       </c>
-      <c r="AD3" t="s">
+      <c r="AF3" t="s">
+        <v>75</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>87</v>
+      </c>
+      <c r="AH3" t="s">
         <v>62</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AF3" t="s">
-        <v>77</v>
-      </c>
-      <c r="AG3" t="s">
-        <v>89</v>
-      </c>
-      <c r="AH3" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:34" ht="17">
@@ -3008,64 +3008,64 @@
         <v>2</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="I4">
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="K4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="L4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="M4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="N4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="O4">
         <v>2</v>
       </c>
       <c r="P4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="Q4">
         <v>2</v>
       </c>
       <c r="R4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="S4" s="7">
         <v>2</v>
       </c>
       <c r="T4" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="U4" s="7">
         <v>2</v>
       </c>
       <c r="V4" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="W4" s="11">
         <v>9</v>
@@ -3080,28 +3080,28 @@
         <v>1</v>
       </c>
       <c r="AA4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="AB4">
         <v>0</v>
       </c>
       <c r="AC4" t="s">
+        <v>59</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE4" t="s">
         <v>61</v>
       </c>
-      <c r="AD4" t="s">
-        <v>62</v>
-      </c>
-      <c r="AE4" t="s">
-        <v>63</v>
-      </c>
       <c r="AF4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="AG4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="AH4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:34" ht="17">
@@ -3112,64 +3112,64 @@
         <v>3</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="F5" t="s">
+        <v>67</v>
+      </c>
+      <c r="G5" t="s">
         <v>54</v>
       </c>
-      <c r="E5" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="F5" t="s">
-        <v>69</v>
-      </c>
-      <c r="G5" t="s">
-        <v>56</v>
-      </c>
       <c r="H5" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="I5">
         <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="K5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="L5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="M5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="N5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="O5">
         <v>3</v>
       </c>
       <c r="P5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="Q5">
         <v>3</v>
       </c>
       <c r="R5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="S5" s="7">
         <v>3</v>
       </c>
       <c r="T5" s="7" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="U5" s="7">
         <v>3</v>
       </c>
       <c r="V5" s="7" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="W5" s="10">
         <v>8</v>
@@ -3184,25 +3184,25 @@
         <v>1</v>
       </c>
       <c r="AA5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="AB5">
         <v>0</v>
       </c>
       <c r="AC5" t="s">
+        <v>59</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE5" t="s">
         <v>61</v>
       </c>
-      <c r="AD5" t="s">
-        <v>62</v>
-      </c>
-      <c r="AE5" t="s">
-        <v>63</v>
-      </c>
       <c r="AF5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="AG5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:34" ht="17">
@@ -3213,64 +3213,64 @@
         <v>4</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="I6">
         <v>1</v>
       </c>
       <c r="J6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="K6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="L6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="M6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="N6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="O6">
         <v>4</v>
       </c>
       <c r="P6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="Q6">
         <v>4</v>
       </c>
       <c r="R6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="S6" s="7">
         <v>4</v>
       </c>
       <c r="T6" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="U6" s="7">
         <v>4</v>
       </c>
       <c r="V6" s="7" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="W6" s="10">
         <v>9</v>
@@ -3285,25 +3285,25 @@
         <v>1</v>
       </c>
       <c r="AA6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="AB6">
         <v>0</v>
       </c>
       <c r="AC6" t="s">
+        <v>59</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE6" t="s">
         <v>61</v>
       </c>
-      <c r="AD6" t="s">
-        <v>62</v>
-      </c>
-      <c r="AE6" t="s">
-        <v>63</v>
-      </c>
       <c r="AF6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="AG6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:34" ht="17">
@@ -3314,64 +3314,64 @@
         <v>5</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="F7" t="s">
+        <v>71</v>
+      </c>
+      <c r="G7" t="s">
         <v>54</v>
       </c>
-      <c r="E7" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="F7" t="s">
-        <v>73</v>
-      </c>
-      <c r="G7" t="s">
-        <v>56</v>
-      </c>
       <c r="H7" s="5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="I7">
         <v>1</v>
       </c>
       <c r="J7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="K7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="L7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="M7" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="N7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="O7">
         <v>5</v>
       </c>
       <c r="P7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="Q7">
         <v>5</v>
       </c>
       <c r="R7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="S7" s="7">
         <v>5</v>
       </c>
       <c r="T7" s="7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="U7" s="7">
         <v>5</v>
       </c>
       <c r="V7" s="7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="W7" s="11">
         <v>9</v>
@@ -3386,25 +3386,25 @@
         <v>1</v>
       </c>
       <c r="AA7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="AB7">
         <v>0</v>
       </c>
       <c r="AC7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE7" t="s">
         <v>61</v>
       </c>
-      <c r="AD7" t="s">
-        <v>62</v>
-      </c>
-      <c r="AE7" t="s">
-        <v>63</v>
-      </c>
       <c r="AF7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="AG7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:34" ht="17">
@@ -3415,64 +3415,64 @@
         <v>6</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="I8">
         <v>1</v>
       </c>
       <c r="J8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="K8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="L8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="M8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="N8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="O8">
         <v>6</v>
       </c>
       <c r="P8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="Q8">
         <v>6</v>
       </c>
       <c r="R8" s="12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="S8" s="7">
         <v>6</v>
       </c>
       <c r="T8" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="U8" s="7">
         <v>6</v>
       </c>
       <c r="V8" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="W8" s="10">
         <v>8</v>
@@ -3487,25 +3487,25 @@
         <v>1</v>
       </c>
       <c r="AA8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="AB8">
         <v>0</v>
       </c>
       <c r="AC8" t="s">
+        <v>59</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE8" t="s">
         <v>61</v>
       </c>
-      <c r="AD8" t="s">
-        <v>62</v>
-      </c>
-      <c r="AE8" t="s">
-        <v>63</v>
-      </c>
       <c r="AF8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="AG8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:34">

</xml_diff>